<commit_message>
Updated order of genes, fixed sept-6 gene, cleaned escape data table
</commit_message>
<xml_diff>
--- a/resources_studies/Cotton2014/ddu564supp_table5_mod.xlsx
+++ b/resources_studies/Cotton2014/ddu564supp_table5_mod.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karinemoussa/Documents/DrLiu_Lab/Shiny_Apps/xci-app-1/resources_studies/Cotton2014/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C05474-DEDD-0443-8CFE-7A58302677EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A43F4C94-B13E-D640-88E0-17807CD085D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="500" windowWidth="32240" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sup Tab 5" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14701" uniqueCount="457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14704" uniqueCount="458">
   <si>
     <t>Closest annotated TSS information</t>
   </si>
@@ -1400,6 +1400,9 @@
   <si>
     <t>NOVEL</t>
   </si>
+  <si>
+    <t>SEPTIN6</t>
+  </si>
 </sst>
 </file>
 
@@ -2233,8 +2236,8 @@
   </sheetPr>
   <dimension ref="A3:AE494"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A339" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B350" sqref="B350"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="11"/>
@@ -34876,8 +34879,8 @@
       <c r="A348" s="9">
         <v>118826791</v>
       </c>
-      <c r="B348" s="10">
-        <v>41158</v>
+      <c r="B348" s="10" t="s">
+        <v>457</v>
       </c>
       <c r="C348" s="11" t="s">
         <v>23</v>
@@ -34971,8 +34974,8 @@
       <c r="A349" s="9">
         <v>118827140</v>
       </c>
-      <c r="B349" s="10">
-        <v>41158</v>
+      <c r="B349" s="10" t="s">
+        <v>457</v>
       </c>
       <c r="C349" s="11" t="s">
         <v>17</v>
@@ -35066,8 +35069,8 @@
       <c r="A350" s="9">
         <v>118827332</v>
       </c>
-      <c r="B350" s="10">
-        <v>41158</v>
+      <c r="B350" s="10" t="s">
+        <v>457</v>
       </c>
       <c r="C350" s="11" t="s">
         <v>17</v>

</xml_diff>